<commit_message>
feat: Actualizado hasta suroeste
</commit_message>
<xml_diff>
--- a/lista municipios.xlsx
+++ b/lista municipios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Esteban\Web Scraping\booking_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C467CF-CEA1-4A35-956C-7BAE34543032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095FA1DD-8F1E-4441-AE37-2D0FE9B21CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1ED7EE49-AFF3-42A1-AA68-204F6DE1AEB3}"/>
   </bookViews>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28124545-FABC-4D6E-8026-0883E6854C94}">
   <dimension ref="A1:F125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
+      <selection activeCell="J93" sqref="J93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
feat: Valle de Aburrá sin Medellín
</commit_message>
<xml_diff>
--- a/lista municipios.xlsx
+++ b/lista municipios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Esteban\Web Scraping\booking_scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD22F9B-A69F-4E94-887C-D73C9C7DAE76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F45AB3-FD8A-460A-854C-0F10E5D432C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{1ED7EE49-AFF3-42A1-AA68-204F6DE1AEB3}"/>
   </bookViews>
@@ -446,7 +446,7 @@
     <t>limpiar datos, puede ser buscar repetidos y quitar los más lejanos la centro</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>revisar municipios</t>
   </si>
 </sst>
 </file>
@@ -973,7 +973,7 @@
   <dimension ref="A1:F125"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A110" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>